<commit_message>
subindo funcionalidade de delete
</commit_message>
<xml_diff>
--- a/docs/Cronograma.xlsx
+++ b/docs/Cronograma.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\judocas\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79C495A6-CD2B-44A3-A3A6-2C8A18D1D3AC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1E33097-319F-4F96-886C-2FEA772FE2E4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{1433F7C8-22CC-4C5C-AA61-3450ABAF355A}"/>
   </bookViews>
@@ -132,9 +132,6 @@
     <t>Implementação de busca para alteração de dados das classes</t>
   </si>
   <si>
-    <t>Testes de homologação relacionados a buscas e alteração dos dados</t>
-  </si>
-  <si>
     <t>Implementação das funcionalidades de atualização dos dados das classes</t>
   </si>
   <si>
@@ -145,6 +142,10 @@
   </si>
   <si>
     <t>Testes de homologação relacionados ao software em geral, para identificação de bugs e erros e correção dos mesmos</t>
+  </si>
+  <si>
+    <t>Mostrar a renovação da carteira de filiação de um aluno/professor com data vencida
+“Promoção” de um aluno a professor</t>
   </si>
 </sst>
 </file>
@@ -267,7 +268,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -781,7 +782,7 @@
   <dimension ref="A1:C14"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -884,7 +885,7 @@
         <v>44122</v>
       </c>
       <c r="B9" s="10" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C9" t="s">
         <v>23</v>
@@ -896,7 +897,7 @@
         <v>44129</v>
       </c>
       <c r="B10" s="10" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C10" t="s">
         <v>24</v>
@@ -908,7 +909,7 @@
         <v>44136</v>
       </c>
       <c r="B11" s="10" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C11" t="s">
         <v>22</v>
@@ -920,19 +921,19 @@
         <v>44143</v>
       </c>
       <c r="B12" s="11" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C12" s="4" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="13" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <f t="shared" si="0"/>
         <v>44150</v>
       </c>
-      <c r="B13" s="10" t="s">
-        <v>34</v>
+      <c r="B13" s="2" t="s">
+        <v>36</v>
       </c>
       <c r="C13" t="s">
         <v>23</v>
@@ -944,7 +945,7 @@
         <v>44157</v>
       </c>
       <c r="B14" s="11" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C14" s="4" t="s">
         <v>25</v>

</xml_diff>

<commit_message>
adcionada listagem de carteiras vencidas
</commit_message>
<xml_diff>
--- a/docs/Cronograma.xlsx
+++ b/docs/Cronograma.xlsx
@@ -8,13 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\judocas\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1E33097-319F-4F96-886C-2FEA772FE2E4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4FF5E0F-285F-48D7-8463-1C07414089D8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{1433F7C8-22CC-4C5C-AA61-3450ABAF355A}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{1433F7C8-22CC-4C5C-AA61-3450ABAF355A}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet1 (2)" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet1 (2)" sheetId="2" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191028"/>
   <extLst>
@@ -34,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="19">
   <si>
     <t>Semana (domingos)</t>
   </si>
@@ -48,60 +47,6 @@
     <t>Análise dos diagramas e eventuais ajustes nos mesmos</t>
   </si>
   <si>
-    <t>Banco de dados implementado conforme o modelo definido anteriormente</t>
-  </si>
-  <si>
-    <t>Banco de dados online, com schemas e tabelas definidos e já alimentado com dados fictícios</t>
-  </si>
-  <si>
-    <t>Desenvolvimento do back end: principais funcionalidades já desenvolvidas, com base nos casos de uso</t>
-  </si>
-  <si>
-    <t>Desenvolvimento do back end: conexão com o banco de dados e criação das classes, conforme o diagrama de classes</t>
-  </si>
-  <si>
-    <t>Desenvolvimento do front end: elaboração do design de telas com base nas funcionalidades criadas no back end</t>
-  </si>
-  <si>
-    <t>Back end funcional e conectado com o banco de dados</t>
-  </si>
-  <si>
-    <t>Desenvolvimento do front end: implementação das funcionalidades projetadas anteriormente</t>
-  </si>
-  <si>
-    <t>Banco de dados, back end e front end já conectados e funcionando localmente</t>
-  </si>
-  <si>
-    <t>Alocação em servidor web e eventuais correções de bugs/ ajustes finais</t>
-  </si>
-  <si>
-    <t>Aplicação funcional e online</t>
-  </si>
-  <si>
-    <t>Linguagem/ferramenta</t>
-  </si>
-  <si>
-    <t>-</t>
-  </si>
-  <si>
-    <t>Banco de dados relacional/ Azure SQLServer</t>
-  </si>
-  <si>
-    <t>Python / Jupyter notebook</t>
-  </si>
-  <si>
-    <t>Azure web apps</t>
-  </si>
-  <si>
-    <t>Todas as anteriores</t>
-  </si>
-  <si>
-    <t>HTML/JavaScript/CSS</t>
-  </si>
-  <si>
-    <t>Conexão entre o back end (já desenvolvido) e o front end através de JSON</t>
-  </si>
-  <si>
     <t>Paulo</t>
   </si>
   <si>
@@ -136,9 +81,6 @@
   </si>
   <si>
     <t>Implementação da funcionalidade de deletar um objeto de uma classe</t>
-  </si>
-  <si>
-    <t>Homologação final do software, visando a correção de todos os erros e bugs identificados</t>
   </si>
   <si>
     <t>Testes de homologação relacionados ao software em geral, para identificação de bugs e erros e correção dos mesmos</t>
@@ -146,6 +88,9 @@
   <si>
     <t>Mostrar a renovação da carteira de filiação de um aluno/professor com data vencida
 “Promoção” de um aluno a professor</t>
+  </si>
+  <si>
+    <t>Homologação final do software, visando a correção de todos os erros e bugs identificados e preenchimento do Cheklist</t>
   </si>
 </sst>
 </file>
@@ -213,24 +158,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="16" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -563,243 +499,28 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D963A5C5-9DB6-4E33-9C38-19C232161330}">
-  <dimension ref="A1:D13"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{07B1BC51-313E-46C5-9107-EEF22B855ED1}">
+  <dimension ref="A1:C14"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="18.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="43.85546875" style="2" customWidth="1"/>
-    <col min="3" max="3" width="33.5703125" style="2" customWidth="1"/>
-    <col min="4" max="4" width="11" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="8" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="D1" s="7" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A2" s="1">
-        <v>44080</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C2" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="D2" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A3" s="1">
-        <f t="shared" ref="A3:A13" si="0">A2+7</f>
-        <v>44087</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="D3" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A4" s="5">
-        <f t="shared" si="0"/>
-        <v>44094</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="D4" s="4" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A5" s="1">
-        <f t="shared" si="0"/>
-        <v>44101</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="D5" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A6" s="1">
-        <f t="shared" si="0"/>
-        <v>44108</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="D6" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A7" s="5">
-        <f t="shared" si="0"/>
-        <v>44115</v>
-      </c>
-      <c r="B7" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="C7" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="D7" s="4" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A8" s="1">
-        <f t="shared" si="0"/>
-        <v>44122</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="D8" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A9" s="1">
-        <f t="shared" si="0"/>
-        <v>44129</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="D9" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A10" s="1">
-        <f t="shared" si="0"/>
-        <v>44136</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="D10" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A11" s="5">
-        <f t="shared" si="0"/>
-        <v>44143</v>
-      </c>
-      <c r="B11" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="C11" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="D11" s="4" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A12" s="1">
-        <f t="shared" si="0"/>
-        <v>44150</v>
-      </c>
-      <c r="B12" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C12" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="D12" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" s="5">
-        <f t="shared" si="0"/>
-        <v>44157</v>
-      </c>
-      <c r="B13" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="C13" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="D13" s="4" t="s">
-        <v>25</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{07B1BC51-313E-46C5-9107-EEF22B855ED1}">
-  <dimension ref="A1:C14"/>
-  <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="18.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="43.85546875" style="10" customWidth="1"/>
+    <col min="2" max="2" width="43.85546875" style="7" customWidth="1"/>
     <col min="3" max="3" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="7" t="s">
+      <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="9" t="s">
+      <c r="B1" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="7" t="s">
+      <c r="C1" s="5" t="s">
         <v>2</v>
       </c>
     </row>
@@ -807,11 +528,11 @@
       <c r="A2" s="1">
         <v>44080</v>
       </c>
-      <c r="B2" s="10" t="s">
+      <c r="B2" s="7" t="s">
         <v>3</v>
       </c>
       <c r="C2" t="s">
-        <v>25</v>
+        <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="30" x14ac:dyDescent="0.25">
@@ -819,40 +540,40 @@
         <f>A2+7</f>
         <v>44087</v>
       </c>
-      <c r="B3" s="10" t="s">
-        <v>26</v>
+      <c r="B3" s="7" t="s">
+        <v>8</v>
       </c>
       <c r="C3" t="s">
-        <v>23</v>
+        <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="33" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="12">
+      <c r="A4" s="9">
         <f>A3+7</f>
         <v>44094</v>
       </c>
-      <c r="B4" s="13" t="s">
-        <v>27</v>
-      </c>
-      <c r="C4" s="14" t="s">
-        <v>22</v>
+      <c r="B4" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" s="11" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="12"/>
-      <c r="B5" s="13"/>
-      <c r="C5" s="14"/>
+      <c r="A5" s="9"/>
+      <c r="B5" s="10"/>
+      <c r="C5" s="11"/>
     </row>
     <row r="6" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <f>A4+7</f>
         <v>44101</v>
       </c>
-      <c r="B6" s="10" t="s">
-        <v>28</v>
+      <c r="B6" s="7" t="s">
+        <v>10</v>
       </c>
       <c r="C6" t="s">
-        <v>24</v>
+        <v>6</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="30" x14ac:dyDescent="0.25">
@@ -860,23 +581,23 @@
         <f t="shared" ref="A7:A14" si="0">A6+7</f>
         <v>44108</v>
       </c>
-      <c r="B7" s="10" t="s">
-        <v>29</v>
+      <c r="B7" s="7" t="s">
+        <v>11</v>
       </c>
       <c r="C7" t="s">
-        <v>22</v>
+        <v>4</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="45" x14ac:dyDescent="0.25">
-      <c r="A8" s="5">
+      <c r="A8" s="4">
         <f t="shared" si="0"/>
         <v>44115</v>
       </c>
-      <c r="B8" s="11" t="s">
-        <v>30</v>
-      </c>
-      <c r="C8" s="4" t="s">
-        <v>25</v>
+      <c r="B8" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="30" x14ac:dyDescent="0.25">
@@ -884,11 +605,11 @@
         <f t="shared" si="0"/>
         <v>44122</v>
       </c>
-      <c r="B9" s="10" t="s">
-        <v>31</v>
+      <c r="B9" s="7" t="s">
+        <v>13</v>
       </c>
       <c r="C9" t="s">
-        <v>23</v>
+        <v>5</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="30" x14ac:dyDescent="0.25">
@@ -896,11 +617,11 @@
         <f t="shared" si="0"/>
         <v>44129</v>
       </c>
-      <c r="B10" s="10" t="s">
-        <v>32</v>
+      <c r="B10" s="7" t="s">
+        <v>14</v>
       </c>
       <c r="C10" t="s">
-        <v>24</v>
+        <v>6</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -908,23 +629,23 @@
         <f t="shared" si="0"/>
         <v>44136</v>
       </c>
-      <c r="B11" s="10" t="s">
-        <v>33</v>
+      <c r="B11" s="7" t="s">
+        <v>15</v>
       </c>
       <c r="C11" t="s">
-        <v>22</v>
+        <v>4</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="45" x14ac:dyDescent="0.25">
-      <c r="A12" s="5">
+      <c r="A12" s="4">
         <f t="shared" si="0"/>
         <v>44143</v>
       </c>
-      <c r="B12" s="11" t="s">
-        <v>35</v>
-      </c>
-      <c r="C12" s="4" t="s">
-        <v>24</v>
+      <c r="B12" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="13" spans="1:3" ht="45" x14ac:dyDescent="0.25">
@@ -933,22 +654,22 @@
         <v>44150</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>36</v>
+        <v>17</v>
       </c>
       <c r="C13" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A14" s="5">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A14" s="4">
         <f t="shared" si="0"/>
         <v>44157</v>
       </c>
-      <c r="B14" s="11" t="s">
-        <v>34</v>
-      </c>
-      <c r="C14" s="4" t="s">
-        <v>25</v>
+      <c r="B14" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>